<commit_message>
support copy worksheet. support add chart. #18 bug fix get_formatted_value. #19
</commit_message>
<xml_diff>
--- a/tests/test_files/aaa.xlsx
+++ b/tests/test_files/aaa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="8175" yWindow="-90" windowWidth="14805" windowHeight="12345" activeTab="5"/>
+    <workbookView xWindow="8175" yWindow="-90" windowWidth="14805" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>trest</t>
     <phoneticPr fontId="1"/>
@@ -436,6 +436,10 @@
   </si>
   <si>
     <t>TEST</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>123456789012345678</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -930,6 +934,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>ライン①</c:v>
+          </c:tx>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$G$7:$G$10</c:f>
@@ -956,6 +963,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>ライン②</c:v>
+          </c:tx>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$H$7:$H$10</c:f>
@@ -989,11 +999,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202541568"/>
-        <c:axId val="203030528"/>
+        <c:axId val="207163904"/>
+        <c:axId val="207356480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202541568"/>
+        <c:axId val="207163904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203030528"/>
+        <c:crossAx val="207356480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,7 +1020,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203030528"/>
+        <c:axId val="207356480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,13 +1031,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202541568"/>
+        <c:crossAx val="207163904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1181,11 +1192,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202495488"/>
-        <c:axId val="173400640"/>
+        <c:axId val="208927744"/>
+        <c:axId val="208610432"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="202495488"/>
+        <c:axId val="208927744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173400640"/>
+        <c:crossAx val="208610432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1203,7 +1214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173400640"/>
+        <c:axId val="208610432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,14 +1225,13 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202495488"/>
+        <c:crossAx val="208927744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1361,11 +1371,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="173402368"/>
-        <c:axId val="173402944"/>
+        <c:axId val="208612160"/>
+        <c:axId val="208612736"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="173402368"/>
+        <c:axId val="208612160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,12 +1385,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173402944"/>
+        <c:crossAx val="208612736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="173402944"/>
+        <c:axId val="208612736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,14 +1401,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173402368"/>
+        <c:crossAx val="208612160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1546,11 +1555,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202876928"/>
-        <c:axId val="203034560"/>
+        <c:axId val="208311808"/>
+        <c:axId val="207359936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202876928"/>
+        <c:axId val="208311808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1568,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203034560"/>
+        <c:crossAx val="207359936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1576,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203034560"/>
+        <c:axId val="207359936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,21 +1584,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202876928"/>
+        <c:crossAx val="208311808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1705,7 +1712,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1809,7 +1815,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1942,11 +1947,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203038016"/>
-        <c:axId val="204439552"/>
+        <c:axId val="208363520"/>
+        <c:axId val="208364096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203038016"/>
+        <c:axId val="208363520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1956,12 +1961,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204439552"/>
+        <c:crossAx val="208364096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="204439552"/>
+        <c:axId val="208364096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1972,7 +1977,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203038016"/>
+        <c:crossAx val="208363520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2045,7 +2050,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2161,11 +2165,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="203597312"/>
-        <c:axId val="204441280"/>
+        <c:axId val="208312832"/>
+        <c:axId val="208365824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="203597312"/>
+        <c:axId val="208312832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2174,7 +2178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204441280"/>
+        <c:crossAx val="208365824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2182,7 +2186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204441280"/>
+        <c:axId val="208365824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,14 +2197,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203597312"/>
+        <c:crossAx val="208312832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2330,12 +2333,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="203597824"/>
-        <c:axId val="204443008"/>
+        <c:axId val="208313344"/>
+        <c:axId val="208367552"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="203597824"/>
+        <c:axId val="208313344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2344,7 +2347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204443008"/>
+        <c:crossAx val="208367552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2352,7 +2355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204443008"/>
+        <c:axId val="208367552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2363,7 +2366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203597824"/>
+        <c:crossAx val="208313344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2520,11 +2523,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="202493952"/>
-        <c:axId val="204444736"/>
+        <c:axId val="208926208"/>
+        <c:axId val="208369280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="202493952"/>
+        <c:axId val="208926208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2533,7 +2536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204444736"/>
+        <c:crossAx val="208369280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2541,7 +2544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204444736"/>
+        <c:axId val="208369280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2552,14 +2555,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202493952"/>
+        <c:crossAx val="208926208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2722,12 +2724,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202494464"/>
-        <c:axId val="204446464"/>
-        <c:axId val="202764928"/>
+        <c:axId val="208926720"/>
+        <c:axId val="208371008"/>
+        <c:axId val="207035520"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="202494464"/>
+        <c:axId val="208926720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2736,7 +2738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204446464"/>
+        <c:crossAx val="208371008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2744,7 +2746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204446464"/>
+        <c:axId val="208371008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2755,12 +2757,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202494464"/>
+        <c:crossAx val="208926720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="202764928"/>
+        <c:axId val="207035520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2769,13 +2771,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204446464"/>
+        <c:crossAx val="208371008"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3832,13 +3833,15 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
     <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="6" width="10.625" customWidth="1"/>
   </cols>
@@ -4090,6 +4093,11 @@
     <row r="35" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B35" s="30">
         <v>1.2344999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B37" s="25" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -4459,7 +4467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed lazy load bug #29 Processing speed improvement #32
</commit_message>
<xml_diff>
--- a/tests/test_files/aaa.xlsx
+++ b/tests/test_files/aaa.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05674B2D-B17E-4027-AC5B-679235C84D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8175" yWindow="-90" windowWidth="14805" windowHeight="12345"/>
+    <workbookView xWindow="6525" yWindow="765" windowWidth="21600" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,17 +19,29 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$K$2</definedName>
     <definedName name="名前">Sheet2!$O$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="F7" authorId="0">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -117,12 +130,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="K27" authorId="0">
+    <comment ref="K27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -153,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>trest</t>
     <phoneticPr fontId="1"/>
@@ -442,11 +455,22 @@
     <t>123456789012345678</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>test2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>test1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>列1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
     <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0.0000_);\(0.0000\)"/>
@@ -907,12 +931,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -959,6 +986,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-11F7-42B7-A007-301720C0FE9B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -988,6 +1020,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-11F7-42B7-A007-301720C0FE9B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1038,7 +1075,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1054,7 +1090,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -1109,6 +1145,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3DCB-4D61-9C69-12F64FAE8360}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1146,6 +1187,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3DCB-4D61-9C69-12F64FAE8360}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1183,6 +1229,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3DCB-4D61-9C69-12F64FAE8360}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1247,7 +1298,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -1360,6 +1411,11 @@
             </c:numRef>
           </c:bubbleSize>
           <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A41D-45B6-9001-26CDF563EF9A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1423,7 +1479,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -1506,6 +1562,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3AB0-40C1-9B09-AA5D01104421}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1544,6 +1605,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3AB0-40C1-9B09-AA5D01104421}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1553,7 +1619,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="208311808"/>
         <c:axId val="207359936"/>
@@ -1612,7 +1677,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -1663,6 +1728,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BDD7-4673-AF62-A30065BBF42F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1697,6 +1767,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BDD7-4673-AF62-A30065BBF42F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1737,7 +1812,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -1799,6 +1874,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A7E4-4FCB-8A32-43ADAC7FD2A3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1850,7 +1930,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -1938,6 +2018,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E82C-476F-ACCD-F3DF66EAF120}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2065,7 +2150,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -2119,6 +2204,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-50B5-4B6E-8C20-5F3051444772}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2154,6 +2244,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-50B5-4B6E-8C20-5F3051444772}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2219,7 +2314,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -2287,6 +2382,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2FFA-4B04-8D7B-8721825115AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2322,6 +2422,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2FFA-4B04-8D7B-8721825115AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2388,7 +2493,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -2442,6 +2547,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F087-4894-AB85-2B1AD7AA0586}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2477,6 +2587,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F087-4894-AB85-2B1AD7AA0586}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2512,6 +2627,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F087-4894-AB85-2B1AD7AA0586}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2577,7 +2697,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -2595,7 +2715,6 @@
       <c:rotX val="15"/>
       <c:rotY val="20"/>
       <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -2645,6 +2764,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6D96-41E6-B0C2-1D7AB5581A93}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2680,6 +2804,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6D96-41E6-B0C2-1D7AB5581A93}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2715,6 +2844,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6D96-41E6-B0C2-1D7AB5581A93}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2808,7 +2942,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1"/>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2838,7 +2978,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="直方体 2"/>
+        <xdr:cNvPr id="3" name="直方体 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2915,7 +3061,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="図 3"/>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2959,7 +3111,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="円/楕円 4"/>
+        <xdr:cNvPr id="5" name="円/楕円 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3019,7 +3177,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="カギ線コネクタ 6"/>
+        <xdr:cNvPr id="7" name="カギ線コネクタ 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="3" idx="4"/>
           <a:endCxn id="5" idx="0"/>
@@ -3072,7 +3236,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="直線矢印コネクタ 8"/>
+        <xdr:cNvPr id="9" name="直線矢印コネクタ 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="3" idx="5"/>
           <a:endCxn id="5" idx="0"/>
@@ -3122,7 +3292,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="カギ線コネクタ 7"/>
+        <xdr:cNvPr id="8" name="カギ線コネクタ 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -3164,7 +3340,13 @@
     <xdr:ext cx="1535484" cy="937629"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="正方形/長方形 5"/>
+        <xdr:cNvPr id="6" name="正方形/長方形 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3250,7 +3432,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1"/>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3280,7 +3468,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2"/>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3310,7 +3504,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="グラフ 3"/>
+        <xdr:cNvPr id="4" name="グラフ 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3340,7 +3540,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="グラフ 5"/>
+        <xdr:cNvPr id="6" name="グラフ 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3370,7 +3576,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="グラフ 6"/>
+        <xdr:cNvPr id="7" name="グラフ 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3400,7 +3612,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="グラフ 7"/>
+        <xdr:cNvPr id="8" name="グラフ 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3435,7 +3653,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1"/>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3465,7 +3689,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2"/>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3495,7 +3725,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="グラフ 3"/>
+        <xdr:cNvPr id="4" name="グラフ 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3525,7 +3761,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="グラフ 4"/>
+        <xdr:cNvPr id="5" name="グラフ 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3541,6 +3783,16 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{569355F1-BEA7-4DC7-A456-7E8F9DA4CE3A}" name="テーブル1" displayName="テーブル1" ref="D39:D41" totalsRowShown="0">
+  <autoFilter ref="D39:D41" xr:uid="{569355F1-BEA7-4DC7-A456-7E8F9DA4CE3A}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{8141DF9E-5CA2-48FD-9F5B-6E27C754C90F}" name="列1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3829,14 +4081,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4080,28 +4332,43 @@
         <v>1.2344999999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="31">
         <v>12345675544</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="29">
         <v>1.2344999999999999</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="30">
         <v>1.2344999999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="25" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:K2"/>
+  <autoFilter ref="A2:K2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B17:D17"/>
   </mergeCells>
@@ -4118,19 +4385,22 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="D8" location="Sheet2!A1" display="リッチテキスト"/>
-    <hyperlink ref="C12" location="Sheet1!A1" display="Sheet1!A1"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D8" location="Sheet2!A1" display="リッチテキスト" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C12" location="Sheet1!A1" display="Sheet1!A1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A4:R27"/>
   <sheetViews>
@@ -4270,7 +4540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -4300,7 +4570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B4:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4398,7 +4668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4464,7 +4734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
@@ -4492,7 +4762,7 @@
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="1.1023622047244095" right="1.1023622047244095" top="0.35433070866141736" bottom="0.35433070866141736" header="0.11811023622047245" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="120" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="120" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;P ページ</oddHeader>
     <oddFooter>&amp;L&amp;B 社外秘&amp;B&amp;C&amp;D&amp;R&amp;P ページ</oddFooter>

</xml_diff>

<commit_message>
Improved accuracy by lazy read. #29 Available Image download, append and change. #35
</commit_message>
<xml_diff>
--- a/tests/test_files/aaa.xlsx
+++ b/tests/test_files/aaa.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05674B2D-B17E-4027-AC5B-679235C84D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B260C347-A3B0-4A3C-B9F0-8DCEEB950DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6525" yWindow="765" windowWidth="21600" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <definedName name="名前">Sheet2!$O$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId7"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -166,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>trest</t>
     <phoneticPr fontId="1"/>
@@ -465,6 +468,18 @@
   </si>
   <si>
     <t>列1</t>
+  </si>
+  <si>
+    <t>行ラベル</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>総計</t>
   </si>
 </sst>
 </file>
@@ -833,7 +848,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -886,6 +901,10 @@
     <xf numFmtId="0" fontId="26" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3785,6 +3804,120 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="作成者" refreshedDate="44636.943484027775" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="2" xr:uid="{77E71A49-E2EF-4ED9-B7AD-D3C42AD32709}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="テーブル1[列1]"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="列1" numFmtId="0">
+      <sharedItems count="2">
+        <s v="test1"/>
+        <s v="test2"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69889868-B65B-4515-9BF1-724F1723CEA0}" name="ピボットテーブル2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F44:F47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12003915-E9D7-4606-B3DA-3B51212BD4C6}" name="ピボットテーブル1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D44:D47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{569355F1-BEA7-4DC7-A456-7E8F9DA4CE3A}" name="テーブル1" displayName="テーブル1" ref="D39:D41" totalsRowShown="0">
   <autoFilter ref="D39:D41" xr:uid="{569355F1-BEA7-4DC7-A456-7E8F9DA4CE3A}"/>
@@ -4085,16 +4218,16 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="19.75" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4236,11 +4369,11 @@
       </c>
     </row>
     <row r="17" spans="2:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B20" s="32">
@@ -4332,39 +4465,71 @@
         <v>1.2344999999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="31">
         <v>12345675544</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B34" s="29">
         <v>1.2344999999999999</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B35" s="30">
         <v>1.2344999999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B37" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.15">
       <c r="D39" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.15">
       <c r="D40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.15">
       <c r="D41" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D44" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D45" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D46" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D47" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="47" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -4385,16 +4550,16 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D8" location="Sheet2!A1" display="リッチテキスト" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C12" location="Sheet1!A1" display="Sheet1!A1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4692,28 +4857,28 @@
       <c r="B2" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="F3" s="47"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="F5" s="47"/>
+      <c r="F5" s="49"/>
     </row>
     <row r="6" spans="1:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F6" s="47"/>
+      <c r="F6" s="49"/>
     </row>
     <row r="7" spans="1:13" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="C7" s="37"/>
-      <c r="F7" s="47"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="11" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="G11" s="39"/>

</xml_diff>

<commit_message>
Minor corrections regarding cell updates and font updates
</commit_message>
<xml_diff>
--- a/tests/test_files/aaa.xlsx
+++ b/tests/test_files/aaa.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126BECBB-5EE9-4C2F-8124-074589A0EB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7CADC4-2B23-4C63-B5BA-622AA48A994B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="1935" windowWidth="15165" windowHeight="13665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$K$2</definedName>
@@ -21,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -169,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>trest</t>
     <phoneticPr fontId="1"/>
@@ -480,6 +481,26 @@
   </si>
   <si>
     <t>総計</t>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -4569,7 +4590,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A4:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4631,7 +4654,7 @@
         <v>164</v>
       </c>
       <c r="U6">
-        <f t="shared" ref="U6:U14" si="0">A5+A6</f>
+        <f t="shared" ref="U6:U12" si="0">A5+A6</f>
         <v>5</v>
       </c>
       <c r="V6">
@@ -4813,6 +4836,12 @@
       <c r="W14" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="U15" t="str">
+        <f>"test" &amp; "テスト"</f>
+        <v>testテスト</v>
       </c>
     </row>
     <row r="27" spans="11:11" x14ac:dyDescent="0.15"/>
@@ -5063,4 +5092,137 @@
     <brk id="9" max="1048575" man="1"/>
   </colBreaks>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6F4B40-44BE-4DD6-A92C-0558C7FFA779}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>